<commit_message>
Correcting the DAQ codes. Working on the 4 thread configuration. Bug to solve: The button doesn't change his name and there's an error when toggling linmot variable.
</commit_message>
<xml_diff>
--- a/ParameterFormat.xlsx
+++ b/ParameterFormat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49053a144a54d517/Escritorio/pyTENG_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmartic\PycharmProjects\pyTENG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{FF914709-4CCC-4B02-BAE5-7DC6295255B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E960DD6F-5051-4658-9527-55954F965F50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9417D87-DCE3-4912-A7BF-86BF276A6C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,10 +253,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,20 +518,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -549,7 +545,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -562,8 +558,9 @@
       <c r="D2" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -574,10 +571,11 @@
         <v>1.2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -590,8 +588,9 @@
       <c r="D4" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -602,10 +601,11 @@
         <v>1.6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -616,10 +616,11 @@
         <v>1.8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -632,8 +633,9 @@
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -644,10 +646,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -660,8 +663,9 @@
       <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -674,8 +678,9 @@
       <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -686,10 +691,11 @@
         <v>2.8</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -702,8 +708,9 @@
       <c r="D12" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -714,10 +721,11 @@
         <v>3.2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -728,10 +736,11 @@
         <v>3.4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -744,8 +753,9 @@
       <c r="D15" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -756,10 +766,11 @@
         <v>3.8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -772,8 +783,9 @@
       <c r="D17" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -786,8 +798,9 @@
       <c r="D18" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -798,10 +811,11 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
@@ -814,8 +828,9 @@
       <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -826,10 +841,11 @@
         <v>4.8</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -840,10 +856,11 @@
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -856,8 +873,9 @@
       <c r="D23" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -868,10 +886,11 @@
         <v>5.4</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -884,8 +903,9 @@
       <c r="D25" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
     </row>
   </sheetData>

</xml_diff>